<commit_message>
Cambio de metodologia y Versionado
</commit_message>
<xml_diff>
--- a/se/metodología/Comparación de Metodologias.xlsx
+++ b/se/metodología/Comparación de Metodologias.xlsx
@@ -837,16 +837,17 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
-    <col min="2" max="7" width="47.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" style="1" customWidth="1"/>
+    <col min="3" max="7" width="47.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -1072,7 +1073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="27" customHeight="1">
+    <row r="13" spans="1:7" ht="42" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>